<commit_message>
Avance 21 Noviembre 2018
</commit_message>
<xml_diff>
--- a/Solución/Aproximación transporte de TSF 30%.xlsx
+++ b/Solución/Aproximación transporte de TSF 30%.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="30% A" sheetId="1" r:id="rId1"/>
     <sheet name="45%" sheetId="2" r:id="rId2"/>
+    <sheet name="Extrapolación de Fd" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,6 +23,44 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+  <si>
+    <t>Interpolaciónde factor de diámetro</t>
+  </si>
+  <si>
+    <t>Datos tabla K</t>
+  </si>
+  <si>
+    <t>https://www.conveyoreng.com/wp-content/uploads/downloads/2013/02/CEMC-Screw-Conveyor-Manual-2.20.pdf</t>
+  </si>
+  <si>
+    <t>Diámetro</t>
+  </si>
+  <si>
+    <t>Ecuación</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>Diámetro deseado (in)</t>
+  </si>
+  <si>
+    <t>Parametros de la ecuación</t>
+  </si>
+  <si>
+    <t>Valor calculado</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -884,6 +923,418 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Extrapolación de Fd'!$A$6:$A$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Extrapolación de Fd'!$B$6:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>940</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5544-45EA-A543-80FC251F34B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="804334672"/>
+        <c:axId val="804335920"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="804334672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="804335920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="804335920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="804334672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -964,6 +1415,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1481,6 +1972,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2049,6 +3056,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2332,7 +3374,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,10 +3459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,6 +3555,220 @@
         <v>553.20000000000005</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>8.6999999999999994E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>3.0972</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <f>$B$14*(B17)^($B$15)</f>
+        <v>8.6999999999999994E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>0.63249999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>1.8576999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <f>$E$7*E10^($E$8)</f>
+        <v>4.8686514557511824</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>42</v>
+      </c>
+      <c r="B18">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>48</v>
+      </c>
+      <c r="B19">
+        <v>940</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>